<commit_message>
Update email automation system with improved contact management and template handling
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,59 +451,65 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>company_name</t>
+          <t>job_title</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>company</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>custom_message</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>sender_name</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>sender_title</t>
+          <t>email_sent_date</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rciii95@gmail.com</t>
+          <t>your.email@example.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RC</t>
+          <t>Your</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sweet Places</t>
+          <t>Your Title</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>This is a test email from The Sweet Places automated system.</t>
+          <t>Your Company</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The Sweet Places Team</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Customer Service</t>
+          <t>Your custom message here.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>failed</t>
         </is>
       </c>
     </row>

</xml_diff>